<commit_message>
Commit all the changes
</commit_message>
<xml_diff>
--- a/SizeChart.xlsx
+++ b/SizeChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyndon_nadel/Documents/spglobal-web-app/spglobal-portal-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0CA19F-540A-8E4A-9C06-E820132E475D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42F3132-2310-5545-945D-F93F577DD5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17020" yWindow="-17500" windowWidth="28800" windowHeight="17500" xr2:uid="{FE701284-5CE4-5A49-BEF2-633E385A5E53}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>Width</t>
   </si>
@@ -62,12 +62,6 @@
     <t>Worked</t>
   </si>
   <si>
-    <t>Font size tests</t>
-  </si>
-  <si>
-    <t>24px — Acceptable</t>
-  </si>
-  <si>
     <t>Logo size</t>
   </si>
   <si>
@@ -93,23 +87,19 @@
   </si>
   <si>
     <t>Text width 70%</t>
+  </si>
+  <si>
+    <t>Canvas margins tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,13 +150,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -183,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -194,11 +184,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -519,19 +507,19 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19.5" style="7" customWidth="1"/>
-    <col min="12" max="12" width="19.5" style="9" customWidth="1"/>
-    <col min="13" max="14" width="17.83203125" customWidth="1"/>
-    <col min="15" max="15" width="22.1640625" customWidth="1"/>
-    <col min="16" max="16" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="8" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.5" style="7" customWidth="1"/>
+    <col min="14" max="15" width="17.83203125" customWidth="1"/>
+    <col min="16" max="16" width="22.1640625" customWidth="1"/>
     <col min="17" max="17" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -542,44 +530,44 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
       <c r="O1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="P1" t="s">
         <v>8</v>
@@ -592,37 +580,37 @@
       <c r="B2" s="1">
         <v>1200</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="10">
+        <v>64</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
         <v>96</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>48</v>
       </c>
-      <c r="E2" s="1">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1">
         <v>64</v>
       </c>
-      <c r="G2" s="1">
-        <v>32</v>
-      </c>
-      <c r="H2" s="1">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1">
+        <v>32</v>
+      </c>
       <c r="J2" s="1">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1">
         <f>A2*B2</f>
         <v>1440000</v>
       </c>
-      <c r="K2" s="2">
-        <v>16</v>
-      </c>
-      <c r="L2" s="13">
-        <v>64</v>
-      </c>
-      <c r="P2" t="s">
-        <v>7</v>
+      <c r="M2" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -632,37 +620,37 @@
       <c r="B3" s="1">
         <v>1080</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="10">
+        <v>64</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
         <v>96</v>
       </c>
-      <c r="D3" s="1">
+      <c r="F3" s="1">
         <v>48</v>
       </c>
-      <c r="E3" s="1">
-        <v>32</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1">
         <v>64</v>
       </c>
-      <c r="G3" s="1">
-        <v>32</v>
-      </c>
-      <c r="H3" s="1">
-        <v>20</v>
-      </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1">
+        <v>32</v>
+      </c>
       <c r="J3" s="1">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1">
         <f>A3*B3</f>
         <v>2073600</v>
       </c>
-      <c r="K3" s="2">
-        <v>16</v>
-      </c>
-      <c r="L3" s="13">
-        <v>64</v>
-      </c>
-      <c r="P3" t="s">
-        <v>7</v>
+      <c r="M3" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -672,37 +660,37 @@
       <c r="B4" s="1">
         <v>1920</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="10">
+        <v>64</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
         <v>96</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F4" s="1">
         <v>48</v>
       </c>
-      <c r="E4" s="1">
-        <v>32</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1">
         <v>64</v>
       </c>
-      <c r="G4" s="1">
-        <v>32</v>
-      </c>
-      <c r="H4" s="1">
-        <v>20</v>
-      </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1">
+        <v>32</v>
+      </c>
       <c r="J4" s="1">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1">
         <f>A4*B4</f>
         <v>2073600</v>
       </c>
-      <c r="K4" s="2">
-        <v>16</v>
-      </c>
-      <c r="L4" s="13">
-        <v>64</v>
-      </c>
-      <c r="P4" t="s">
-        <v>7</v>
+      <c r="M4" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -712,37 +700,37 @@
       <c r="B5" s="2">
         <v>420</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
+        <v>32</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
         <v>64</v>
       </c>
-      <c r="D5" s="2">
-        <v>32</v>
-      </c>
-      <c r="E5" s="2">
-        <v>20</v>
-      </c>
       <c r="F5" s="2">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2">
         <v>48</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <v>24</v>
       </c>
-      <c r="H5" s="2">
-        <v>20</v>
-      </c>
-      <c r="I5" s="2"/>
       <c r="J5" s="2">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2">
         <f>A5*B5</f>
         <v>806400</v>
       </c>
-      <c r="K5" s="5">
+      <c r="M5" s="5">
         <v>8</v>
-      </c>
-      <c r="L5" s="4">
-        <v>32</v>
-      </c>
-      <c r="P5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -752,37 +740,37 @@
       <c r="B6" s="2">
         <v>628</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2">
         <v>64</v>
       </c>
-      <c r="D6" s="2">
-        <v>32</v>
-      </c>
-      <c r="E6" s="2">
-        <v>20</v>
-      </c>
       <c r="F6" s="2">
+        <v>32</v>
+      </c>
+      <c r="G6" s="2">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2">
         <v>48</v>
       </c>
-      <c r="G6" s="2">
+      <c r="I6" s="2">
         <v>24</v>
       </c>
-      <c r="H6" s="2">
-        <v>20</v>
-      </c>
-      <c r="I6" s="2"/>
       <c r="J6" s="2">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2">
         <f>A6*B6</f>
         <v>753600</v>
       </c>
-      <c r="K6" s="2">
-        <v>16</v>
-      </c>
-      <c r="L6" s="4">
-        <v>32</v>
-      </c>
-      <c r="P6" t="s">
-        <v>7</v>
+      <c r="M6" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -792,37 +780,37 @@
       <c r="B7" s="2">
         <v>1200</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
+        <v>32</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2">
         <v>64</v>
       </c>
-      <c r="D7" s="2">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2">
-        <v>20</v>
-      </c>
       <c r="F7" s="2">
+        <v>32</v>
+      </c>
+      <c r="G7" s="2">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2">
         <v>48</v>
       </c>
-      <c r="G7" s="2">
+      <c r="I7" s="2">
         <v>24</v>
       </c>
-      <c r="H7" s="2">
-        <v>20</v>
-      </c>
-      <c r="I7" s="2"/>
       <c r="J7" s="2">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
         <f>A7*B7</f>
         <v>753600</v>
       </c>
-      <c r="K7" s="2">
-        <v>16</v>
-      </c>
-      <c r="L7" s="4">
-        <v>32</v>
-      </c>
-      <c r="P7" t="s">
-        <v>7</v>
+      <c r="M7" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -832,37 +820,37 @@
       <c r="B8" s="3">
         <v>300</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3">
         <v>48</v>
       </c>
-      <c r="D8" s="3">
+      <c r="F8" s="3">
         <v>24</v>
       </c>
-      <c r="E8" s="3">
-        <v>20</v>
-      </c>
-      <c r="F8" s="3">
-        <v>32</v>
-      </c>
       <c r="G8" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H8" s="3">
-        <v>20</v>
-      </c>
-      <c r="I8" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="I8" s="3">
+        <v>16</v>
+      </c>
       <c r="J8" s="3">
+        <v>20</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3">
         <f>A8*B8</f>
         <v>450000</v>
       </c>
-      <c r="K8" s="5">
+      <c r="M8" s="5">
         <v>8</v>
-      </c>
-      <c r="L8" s="4">
-        <v>32</v>
-      </c>
-      <c r="P8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -872,37 +860,37 @@
       <c r="B9" s="3">
         <v>300</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
+        <v>32</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3">
         <v>48</v>
       </c>
-      <c r="D9" s="3">
+      <c r="F9" s="3">
         <v>24</v>
       </c>
-      <c r="E9" s="3">
-        <v>20</v>
-      </c>
-      <c r="F9" s="3">
-        <v>32</v>
-      </c>
       <c r="G9" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H9" s="3">
-        <v>20</v>
-      </c>
-      <c r="I9" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="I9" s="3">
+        <v>16</v>
+      </c>
       <c r="J9" s="3">
+        <v>20</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3">
         <f>A9*B9</f>
         <v>540000</v>
       </c>
-      <c r="K9" s="5">
+      <c r="M9" s="5">
         <v>8</v>
-      </c>
-      <c r="L9" s="4">
-        <v>32</v>
-      </c>
-      <c r="P9" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -912,37 +900,37 @@
       <c r="B10" s="4">
         <v>250</v>
       </c>
-      <c r="C10" s="4">
-        <v>32</v>
-      </c>
-      <c r="D10" s="4">
-        <v>16</v>
+      <c r="C10" s="2">
+        <v>16</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E10" s="4">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F10" s="4">
+        <v>16</v>
+      </c>
+      <c r="G10" s="4">
+        <v>12</v>
+      </c>
+      <c r="H10" s="4">
         <v>24</v>
       </c>
-      <c r="G10" s="4">
+      <c r="I10" s="4">
         <v>14</v>
       </c>
-      <c r="H10" s="4">
-        <v>12</v>
-      </c>
-      <c r="I10" s="4"/>
       <c r="J10" s="4">
+        <v>12</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
         <f>A10*B10</f>
         <v>75000</v>
       </c>
-      <c r="K10" s="5">
+      <c r="M10" s="5">
         <v>8</v>
-      </c>
-      <c r="L10" s="2">
-        <v>16</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -952,37 +940,37 @@
       <c r="B11" s="4">
         <v>205</v>
       </c>
-      <c r="C11" s="4">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4">
-        <v>16</v>
+      <c r="C11" s="2">
+        <v>16</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E11" s="4">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F11" s="4">
+        <v>16</v>
+      </c>
+      <c r="G11" s="4">
+        <v>12</v>
+      </c>
+      <c r="H11" s="4">
         <v>24</v>
       </c>
-      <c r="G11" s="4">
+      <c r="I11" s="4">
         <v>14</v>
       </c>
-      <c r="H11" s="4">
-        <v>12</v>
-      </c>
-      <c r="I11" s="4"/>
       <c r="J11" s="4">
+        <v>12</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
         <f>A11*B11</f>
         <v>126280</v>
       </c>
-      <c r="K11" s="5">
+      <c r="M11" s="5">
         <v>8</v>
-      </c>
-      <c r="L11" s="2">
-        <v>16</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -992,37 +980,37 @@
       <c r="B12" s="4">
         <v>600</v>
       </c>
-      <c r="C12" s="4">
-        <v>32</v>
-      </c>
-      <c r="D12" s="4">
-        <v>16</v>
+      <c r="C12" s="2">
+        <v>16</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E12" s="4">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F12" s="4">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4">
+        <v>12</v>
+      </c>
+      <c r="H12" s="4">
         <v>24</v>
       </c>
-      <c r="G12" s="4">
+      <c r="I12" s="4">
         <v>14</v>
       </c>
-      <c r="H12" s="4">
-        <v>12</v>
-      </c>
-      <c r="I12" s="4"/>
       <c r="J12" s="4">
+        <v>12</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4">
         <f>A12*B12</f>
         <v>180000</v>
       </c>
-      <c r="K12" s="5">
+      <c r="M12" s="5">
         <v>8</v>
-      </c>
-      <c r="L12" s="2">
-        <v>16</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -1032,39 +1020,39 @@
       <c r="B13" s="4">
         <v>180</v>
       </c>
-      <c r="C13" s="4">
-        <v>32</v>
-      </c>
-      <c r="D13" s="4">
-        <v>16</v>
+      <c r="C13" s="2">
+        <v>16</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E13" s="4">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F13" s="4">
+        <v>16</v>
+      </c>
+      <c r="G13" s="4">
+        <v>12</v>
+      </c>
+      <c r="H13" s="4">
         <v>24</v>
       </c>
-      <c r="G13" s="4">
+      <c r="I13" s="4">
         <v>14</v>
       </c>
-      <c r="H13" s="4">
-        <v>12</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4">
+        <v>12</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="4">
+      <c r="L13" s="4">
         <f>A13*B13</f>
         <v>219600</v>
       </c>
-      <c r="K13" s="5">
+      <c r="M13" s="5">
         <v>8</v>
-      </c>
-      <c r="L13" s="2">
-        <v>16</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1074,37 +1062,37 @@
       <c r="B14" s="5">
         <v>150</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="11">
+        <v>12</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5">
         <v>24</v>
       </c>
-      <c r="D14" s="5">
+      <c r="F14" s="5">
         <v>14</v>
       </c>
-      <c r="E14" s="5">
-        <v>12</v>
-      </c>
-      <c r="F14" s="5">
-        <v>20</v>
-      </c>
       <c r="G14" s="5">
         <v>12</v>
       </c>
       <c r="H14" s="5">
-        <v>12</v>
-      </c>
-      <c r="I14" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="I14" s="5">
+        <v>12</v>
+      </c>
       <c r="J14" s="5">
+        <v>12</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5">
         <f>A14*B14</f>
         <v>90000</v>
       </c>
-      <c r="K14" s="5">
+      <c r="M14" s="5">
         <v>8</v>
-      </c>
-      <c r="L14" s="2">
-        <v>16</v>
-      </c>
-      <c r="P14" s="10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1114,39 +1102,39 @@
       <c r="B15" s="5">
         <v>120</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="11">
+        <v>12</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="5">
         <v>24</v>
       </c>
-      <c r="D15" s="5">
+      <c r="F15" s="5">
         <v>14</v>
       </c>
-      <c r="E15" s="5">
-        <v>12</v>
-      </c>
-      <c r="F15" s="5">
-        <v>20</v>
-      </c>
       <c r="G15" s="5">
         <v>12</v>
       </c>
       <c r="H15" s="5">
-        <v>12</v>
-      </c>
-      <c r="I15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="5">
+        <v>12</v>
+      </c>
+      <c r="J15" s="5">
+        <v>12</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="5">
+      <c r="L15" s="5">
         <f>A15*B15</f>
         <v>118800</v>
       </c>
-      <c r="K15" s="5">
+      <c r="M15" s="5">
         <v>8</v>
-      </c>
-      <c r="L15" s="2">
-        <v>16</v>
-      </c>
-      <c r="P15" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -1156,127 +1144,124 @@
       <c r="B16" s="5">
         <v>600</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="11">
+        <v>12</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="5">
         <v>24</v>
       </c>
-      <c r="D16" s="5">
+      <c r="F16" s="5">
         <v>14</v>
       </c>
-      <c r="E16" s="5">
-        <v>12</v>
-      </c>
-      <c r="F16" s="5">
-        <v>20</v>
-      </c>
       <c r="G16" s="5">
         <v>12</v>
       </c>
       <c r="H16" s="5">
-        <v>12</v>
-      </c>
-      <c r="I16" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="I16" s="5">
+        <v>12</v>
+      </c>
       <c r="J16" s="5">
+        <v>12</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5">
         <f>A16*B16</f>
         <v>96000</v>
       </c>
-      <c r="K16" s="5">
+      <c r="M16" s="5">
         <v>8</v>
       </c>
-      <c r="L16" s="12">
-        <v>12</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>400</v>
       </c>
       <c r="B17" s="6">
         <v>100</v>
       </c>
-      <c r="C17" s="6">
-        <v>20</v>
-      </c>
-      <c r="D17" s="6">
-        <v>12</v>
+      <c r="C17" s="11">
+        <v>12</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E17" s="6">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F17" s="6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G17" s="6">
         <v>12</v>
       </c>
       <c r="H17" s="6">
-        <v>12</v>
-      </c>
-      <c r="I17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="6">
+        <v>12</v>
+      </c>
+      <c r="J17" s="6">
+        <v>12</v>
+      </c>
+      <c r="K17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="6">
+      <c r="L17" s="6">
         <f>A17*B17</f>
         <v>40000</v>
       </c>
-      <c r="K17" s="4">
+      <c r="M17" s="4">
         <v>4</v>
       </c>
-      <c r="L17" s="12">
-        <v>12</v>
-      </c>
-      <c r="P17" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>728</v>
       </c>
       <c r="B18" s="6">
         <v>90</v>
       </c>
-      <c r="C18" s="6">
-        <v>20</v>
-      </c>
-      <c r="D18" s="6">
-        <v>12</v>
+      <c r="C18" s="11">
+        <v>12</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E18" s="6">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F18" s="6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G18" s="6">
         <v>12</v>
       </c>
       <c r="H18" s="6">
-        <v>12</v>
-      </c>
-      <c r="I18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="6">
+        <v>12</v>
+      </c>
+      <c r="J18" s="6">
+        <v>12</v>
+      </c>
+      <c r="K18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="6">
+      <c r="L18" s="6">
         <f>A18*B18</f>
         <v>65520</v>
       </c>
-      <c r="K18" s="4">
+      <c r="M18" s="4">
         <v>4</v>
       </c>
-      <c r="L18" s="12">
-        <v>12</v>
-      </c>
-      <c r="P18" s="8" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P19">
-    <sortCondition descending="1" ref="L1:L19"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>